<commit_message>
update LF-condition_ pattern emerges and disappears now
</commit_message>
<xml_diff>
--- a/simulated_data/dyads_simulated/cond2_leader_follower/HRV_B.xlsx
+++ b/simulated_data/dyads_simulated/cond2_leader_follower/HRV_B.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A692"/>
+  <dimension ref="A1:A700"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,3452 +435,3492 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>603.099603413507</v>
+        <v>549.2624508253945</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>581.6162752718639</v>
+        <v>502.8699661021523</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>601.6425595070502</v>
+        <v>531.0838140062446</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>634.2515626198224</v>
+        <v>598.2882260105345</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>655.5714120838019</v>
+        <v>670.7275132871837</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>674.0804630719217</v>
+        <v>699.677348429669</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>706.5838474674329</v>
+        <v>709.8251599466705</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>611.9855810644603</v>
+        <v>726.0801777708306</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>614.9877560111685</v>
+        <v>681.7092179497974</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>530.3888166776618</v>
+        <v>639.5911145694706</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>504.5425367196037</v>
+        <v>663.4777259788001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>478.4754321871461</v>
+        <v>644.6862563137437</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>471.9073079326544</v>
+        <v>698.3086415910807</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>494.3615817331386</v>
+        <v>725.8656299775553</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>543.3792776705531</v>
+        <v>752.0555883941871</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>614.3709244701388</v>
+        <v>742.6169494921187</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>676.6948287264559</v>
+        <v>667.5355872089366</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>695.0144034642989</v>
+        <v>625.6959244050399</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>679.0300143278056</v>
+        <v>623.1396665675763</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>652.0276523917463</v>
+        <v>582.2371209118255</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>633.0414267661464</v>
+        <v>575.3515768981749</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>609.5906042183401</v>
+        <v>557.5784781004315</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>572.7786360094651</v>
+        <v>513.7577355206382</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>535.1011912389882</v>
+        <v>568.2497142181795</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>504.8814445175029</v>
+        <v>618.1929404620519</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>492.0237316502743</v>
+        <v>623.9199071081387</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>476.6720572754562</v>
+        <v>755.167643709445</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>464.8648635018002</v>
+        <v>790.3040659374553</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>501.4662850230565</v>
+        <v>744.5850178628248</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>519.511072607255</v>
+        <v>652.901965621048</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>504.7745740844398</v>
+        <v>668.4027498268712</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>525.8900791775716</v>
+        <v>635.1936996879352</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>561.6711815746883</v>
+        <v>615.8730909933681</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>592.7046038707289</v>
+        <v>578.746037124862</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>659.7013271279479</v>
+        <v>644.1484238790913</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>660.0405230371784</v>
+        <v>697.1445231719038</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>612.9395854232342</v>
+        <v>685.8890265647979</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>579.1901128922348</v>
+        <v>668.0558472713933</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>628.4842207194074</v>
+        <v>639.5188885037122</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>665.51749696184</v>
+        <v>659.1039683504966</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>647.4762251701769</v>
+        <v>651.3373025105089</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>635.4682632476454</v>
+        <v>606.8615076523862</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>637.3351633715245</v>
+        <v>641.642823987489</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>661.9015682388465</v>
+        <v>601.1015349588291</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>664.3937726496141</v>
+        <v>584.2538564440111</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>648.0600680410973</v>
+        <v>602.0560307258194</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>657.188156497675</v>
+        <v>650.4269929854836</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>628.4171177502565</v>
+        <v>651.0677344578362</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>614.0855784574342</v>
+        <v>635.8447631430017</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>584.5620763895347</v>
+        <v>615.8659216407436</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>557.2691640119309</v>
+        <v>558.4421115605026</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>546.9494753789803</v>
+        <v>560.2782731404687</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>571.0449156105817</v>
+        <v>522.588339278272</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>612.2640398244386</v>
+        <v>587.6964078937235</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>606.3053299696505</v>
+        <v>715.6688571225942</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>552.4561794375913</v>
+        <v>793.7037823166264</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>492.1472642120648</v>
+        <v>731.0672550759919</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>564.5752621782592</v>
+        <v>596.8871015405881</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>656.2277041044879</v>
+        <v>542.3210318236399</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>631.759980631756</v>
+        <v>505.4876226222191</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>605.7910084868538</v>
+        <v>486.073034341473</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>608.4648671319144</v>
+        <v>485.5318994682705</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>599.4540934414658</v>
+        <v>468.3601761099041</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>631.8052259276214</v>
+        <v>464.401563718063</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>674.6310676309761</v>
+        <v>475.0679392023258</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>700.0963451952344</v>
+        <v>533.1286767860845</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>637.9297986777601</v>
+        <v>567.7697578950927</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>602.0490761139924</v>
+        <v>600.9701245232861</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>630.5864125461439</v>
+        <v>648.1657110261879</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>662.032882019048</v>
+        <v>643.4560948411985</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>690.9768784207486</v>
+        <v>678.1480365327823</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>679.8755841832999</v>
+        <v>694.5482625260695</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>623.5472230925225</v>
+        <v>693.3974483362349</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>653.0354148996978</v>
+        <v>637.5396060257543</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>651.3860706033724</v>
+        <v>558.8782007698683</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>652.5118002347199</v>
+        <v>522.5299274943183</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>652.2829655860889</v>
+        <v>507.0215838347281</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>647.6222567487682</v>
+        <v>458.8780110955568</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>686.9673761094291</v>
+        <v>470.6371113505625</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>692.2187538447702</v>
+        <v>500.3207025039629</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>672.6687712616695</v>
+        <v>569.072948606994</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>691.1630111511115</v>
+        <v>629.8270742515655</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>709.9619864246235</v>
+        <v>680.3664381304557</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>712.1286868888817</v>
+        <v>708.9094738603308</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>688.7238579483466</v>
+        <v>689.4184070478389</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>634.0701746130221</v>
+        <v>638.618556321667</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>548.3189288449921</v>
+        <v>597.7717364401656</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>503.3671251955312</v>
+        <v>517.7454367778366</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>479.0203667664059</v>
+        <v>463.9738290064628</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>468.3835873423234</v>
+        <v>417.5301210703211</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>460.4637582660587</v>
+        <v>409.9558195159929</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>423.6776054910152</v>
+        <v>420.0898333335488</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>428.798772069527</v>
+        <v>455.6364364174783</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>567.6610955815988</v>
+        <v>535.1339762169545</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>759.2765955190686</v>
+        <v>615.4124224189843</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>773.5876365963037</v>
+        <v>626.746415592386</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>760.1765544553202</v>
+        <v>671.6687291887879</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>788.634777287733</v>
+        <v>646.4218181570374</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>787.2609263274696</v>
+        <v>607.7404602373662</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>748.2199569248564</v>
+        <v>592.3136667030349</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>678.4187453192985</v>
+        <v>593.6010460086152</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>644.1416985870774</v>
+        <v>604.3124023404545</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>689.3872692154659</v>
+        <v>623.1022004272688</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>734.5614095868456</v>
+        <v>600.0125901871841</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>702.8714024914464</v>
+        <v>574.8934688839072</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>643.126188210104</v>
+        <v>559.8050657145918</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>616.6244505065492</v>
+        <v>569.4287623200864</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>648.1317338764114</v>
+        <v>555.5171956670506</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>684.2251172563891</v>
+        <v>540.9571112605107</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>678.3090087267567</v>
+        <v>514.3940585728757</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>674.6142472600098</v>
+        <v>536.1810772006947</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>661.2565121026108</v>
+        <v>540.3994342207739</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>668.4870156990144</v>
+        <v>636.2403998286368</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>681.5378999558561</v>
+        <v>684.9933122256573</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>700.3502256434899</v>
+        <v>589.2299743018725</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>675.099793675173</v>
+        <v>541.4078844050891</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>658.7171814658461</v>
+        <v>536.7214143521011</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>704.9796721603911</v>
+        <v>524.4249706441053</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>745.8420698085604</v>
+        <v>557.5377477191665</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>779.093818177472</v>
+        <v>633.0888192508581</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>743.5489163188009</v>
+        <v>718.4549306466437</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>681.532655967473</v>
+        <v>762.4958859647677</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>660.885145122009</v>
+        <v>767.6826637308665</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>716.6536142237305</v>
+        <v>720.2111640442581</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>793.0818744732733</v>
+        <v>716.8954834444463</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>804.5262225684837</v>
+        <v>718.8214133315967</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>748.3569176558973</v>
+        <v>739.2425269825225</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>680.2531162369405</v>
+        <v>791.1799994904953</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>687.7352396265763</v>
+        <v>776.7023538392976</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>651.1375700346349</v>
+        <v>783.1618270056708</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>558.3367903131062</v>
+        <v>740.7711627202218</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>531.2280320180349</v>
+        <v>747.4429437155976</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>595.8564456478399</v>
+        <v>716.5924119374125</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>711.0392843999591</v>
+        <v>658.003973154635</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>725.7232791553889</v>
+        <v>662.4377042525111</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>704.8979294924607</v>
+        <v>689.6335912882705</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>689.4684452033033</v>
+        <v>735.9409719834815</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>626.0932106879551</v>
+        <v>668.0061090011691</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>536.1605854118352</v>
+        <v>567.4097680130217</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>520.1849424579876</v>
+        <v>505.1199122413834</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>537.4377975184643</v>
+        <v>503.3000666577578</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>546.9545953284012</v>
+        <v>501.5519497444814</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>558.1769482467394</v>
+        <v>574.5057099901629</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>572.3497190152216</v>
+        <v>693.395835655906</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>592.1894358754685</v>
+        <v>759.8666234832478</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>581.5148249987629</v>
+        <v>771.5138621916537</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>595.8631998566659</v>
+        <v>748.326556176508</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>616.4766583741539</v>
+        <v>646.6281595895964</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>632.9510465471486</v>
+        <v>596.861477161184</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>664.6666860647628</v>
+        <v>585.7709915781157</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>647.9614013670982</v>
+        <v>615.2843689788625</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>630.9615586436905</v>
+        <v>640.9922493415365</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>616.906562050886</v>
+        <v>566.8138137723844</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>600.5400201010787</v>
+        <v>582.4099811087819</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>609.4981856270607</v>
+        <v>604.4298420716245</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>607.7029511817216</v>
+        <v>632.6590597215613</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>584.8872833529413</v>
+        <v>718.6381728512572</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>556.8943709561722</v>
+        <v>739.3865555424384</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>543.5469623397466</v>
+        <v>714.7370998050917</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>502.6249038456001</v>
+        <v>720.2016285043982</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>473.5951788754278</v>
+        <v>624.8480055308931</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>477.5486208241659</v>
+        <v>561.7319953650082</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>503.4676149309263</v>
+        <v>605.2697184397005</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>522.4294831256202</v>
+        <v>651.7594023789712</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>539.931188849522</v>
+        <v>661.4794832330375</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>549.1626776994565</v>
+        <v>691.9550937668077</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>545.1876036008372</v>
+        <v>693.0055832624191</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>527.9911846055114</v>
+        <v>613.3427729609764</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>536.8530808334668</v>
+        <v>597.1362947759928</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>581.7592403722642</v>
+        <v>650.415264498335</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>589.4543708285056</v>
+        <v>647.6703418482117</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>613.0565379759076</v>
+        <v>608.3864725751482</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>638.4767568709009</v>
+        <v>569.3547735809545</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>622.3282701343607</v>
+        <v>532.1633494287425</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>592.224197896968</v>
+        <v>489.2526048136148</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>558.3803228773263</v>
+        <v>486.2327245711242</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>518.923512294549</v>
+        <v>509.7532012703141</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>485.2945430754545</v>
+        <v>586.5357476311601</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>481.6574186483393</v>
+        <v>682.8766893753482</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>499.0099962485885</v>
+        <v>775.2116486898046</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>540.0183021989164</v>
+        <v>794.0867426941054</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>606.0009095386363</v>
+        <v>754.3116409992763</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>707.1328448169254</v>
+        <v>716.4128610344136</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>744.6175799255741</v>
+        <v>695.2957433734639</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>753.5959677231006</v>
+        <v>588.9296498632746</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>740.5759087342147</v>
+        <v>484.7989447749086</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>638.3289273605897</v>
+        <v>438.5386738412222</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>532.4174353084601</v>
+        <v>484.9111935211852</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>479.5323055446801</v>
+        <v>565.9675003537643</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>506.5603683220843</v>
+        <v>655.8519333962494</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>577.7824108011345</v>
+        <v>663.7029677840474</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>612.845717003438</v>
+        <v>659.8263441703551</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>618.7977265007731</v>
+        <v>696.9679603722057</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>625.2062389989703</v>
+        <v>721.3695859725107</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>658.7971354065871</v>
+        <v>683.8754456184688</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>664.1480533806572</v>
+        <v>646.1237382300027</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>645.3618888507435</v>
+        <v>571.8263151921406</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>583.5337933203419</v>
+        <v>526.109057195967</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>513.1802635542755</v>
+        <v>488.19505979246</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>471.710114657256</v>
+        <v>522.4270749569087</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>445.9895245155678</v>
+        <v>514.9911914838441</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>455.4415133581529</v>
+        <v>516.0425232377719</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>460.0346375852524</v>
+        <v>505.9797018562477</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>450.716656213217</v>
+        <v>545.9710939086477</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>452.5088915318776</v>
+        <v>611.6982065164649</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>479.0796212737689</v>
+        <v>648.0896795233093</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>538.974593287378</v>
+        <v>632.6802178486162</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>590.4808489015494</v>
+        <v>610.0839123114099</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>604.0503331715996</v>
+        <v>595.4641687157789</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>606.7797127824264</v>
+        <v>591.8195059201707</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>630.4857311348826</v>
+        <v>555.3545811395395</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>655.0019374735143</v>
+        <v>501.9108933186374</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>615.2596473060328</v>
+        <v>501.7720860019779</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>556.3174181539239</v>
+        <v>503.9815195943049</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>551.6155364531699</v>
+        <v>507.2930035674403</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>559.3485404252192</v>
+        <v>511.6031548945159</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>572.0743281216301</v>
+        <v>509.3628290576078</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>594.6292889891538</v>
+        <v>550.1877861200626</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>593.2344541971588</v>
+        <v>535.2632372683672</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>603.8479820522866</v>
+        <v>566.5706306199354</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>585.6470088049548</v>
+        <v>576.573652142315</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>596.2231903818633</v>
+        <v>595.9231315357272</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>602.6035724414385</v>
+        <v>614.1278605890648</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>607.0279472276638</v>
+        <v>594.2268718301023</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>605.3811861303586</v>
+        <v>585.1441455916699</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>608.349781115237</v>
+        <v>622.3599875576724</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>593.5416942685094</v>
+        <v>562.5769229398543</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>571.7813356015711</v>
+        <v>547.1832961981704</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>512.9054102388579</v>
+        <v>549.4352788534229</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>491.3508475690946</v>
+        <v>590.7230555447427</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>486.2814733865264</v>
+        <v>584.4827083896575</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>520.6519660757465</v>
+        <v>614.812457314855</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>570.8396784961565</v>
+        <v>542.8456453619788</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>652.7412979850453</v>
+        <v>498.2305599738766</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>656.1694825824986</v>
+        <v>471.8115791459638</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>581.6826471515242</v>
+        <v>450.9592888566942</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>518.5617495146175</v>
+        <v>449.3829573687833</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>500.1436527743977</v>
+        <v>498.7686157969335</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>500.2602203281299</v>
+        <v>541.8121421673163</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>511.3724358805314</v>
+        <v>515.7728529912333</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>491.4696922877795</v>
+        <v>506.2585943877309</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>496.2020353491425</v>
+        <v>514.3071410393816</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>556.0457116561111</v>
+        <v>563.7262498920279</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>626.0174992533791</v>
+        <v>648.5627328582098</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>630.9461879311584</v>
+        <v>760.8218298819054</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>682.5590297597444</v>
+        <v>721.1360400025626</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>694.4790018566493</v>
+        <v>660.4775760375503</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>601.9260601247822</v>
+        <v>671.8832685248231</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>611.1247343081914</v>
+        <v>624.0706519761545</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>618.5272810417928</v>
+        <v>551.7115057074875</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>623.7737038610192</v>
+        <v>516.9572088704228</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>625.7094693708325</v>
+        <v>536.9205149601441</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>638.0878895574256</v>
+        <v>638.0820948453731</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>689.8532452149766</v>
+        <v>648.9784879855449</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>701.618588506534</v>
+        <v>633.7605421533965</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>672.6147819266259</v>
+        <v>645.7417169162909</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>654.5375712401835</v>
+        <v>602.414640191995</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>612.0249615831597</v>
+        <v>535.6742951767046</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>550.3363097785723</v>
+        <v>532.6176804429679</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>520.3540217094087</v>
+        <v>540.3814312880968</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>508.2833061562155</v>
+        <v>549.3577241527134</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>506.6369280039282</v>
+        <v>604.705383254867</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>557.1916713265637</v>
+        <v>690.8164526643361</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>659.2796204538161</v>
+        <v>754.5184300302594</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>758.7083359731537</v>
+        <v>728.7163727206689</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>712.8479679604709</v>
+        <v>750.7814583930497</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>718.6815044750006</v>
+        <v>740.5126822519321</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>733.9333668845427</v>
+        <v>663.1751473254894</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>702.9885640010889</v>
+        <v>589.0607895346989</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>658.7698615109332</v>
+        <v>570.0827149572092</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>627.7586024242225</v>
+        <v>607.1928965114353</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>651.0651212573748</v>
+        <v>584.3237108426536</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>606.7395785236727</v>
+        <v>547.7341575604839</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>535.3101874557922</v>
+        <v>570.7711179944965</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>528.9995482550864</v>
+        <v>580.7638930066616</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>518.7123171818371</v>
+        <v>561.9498473143096</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>493.3541915463593</v>
+        <v>630.8302131472487</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>528.4143170186724</v>
+        <v>758.8606754413547</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>682.6352162726721</v>
+        <v>783.2956137270628</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>769.448759157342</v>
+        <v>824.8987689945864</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>786.0896348097128</v>
+        <v>826.5035964382434</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>819.211686509135</v>
+        <v>831.1675208894655</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>817.1848981891117</v>
+        <v>734.4330656788145</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>766.9610117011132</v>
+        <v>740.3649858807171</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>682.3788238457382</v>
+        <v>732.0019419392736</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>699.7978225578834</v>
+        <v>746.478450286105</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>716.9783649777344</v>
+        <v>762.7258812550508</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>756.9047217245384</v>
+        <v>754.8956768568473</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>779.7049079377985</v>
+        <v>743.3822620166382</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>751.4420718417512</v>
+        <v>675.5856162927785</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>714.2272932701417</v>
+        <v>661.7254951854648</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>642.6466542735056</v>
+        <v>682.4251081579291</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>653.5668447406522</v>
+        <v>682.4579968553621</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>667.3736843897871</v>
+        <v>682.6665545017363</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>680.0621531046431</v>
+        <v>624.6642079126161</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>671.9308193449081</v>
+        <v>627.2354077160287</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>605.9665205898739</v>
+        <v>682.5541305383922</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>633.4358544200995</v>
+        <v>728.10893619436</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>681.2420049956529</v>
+        <v>766.095051472405</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>721.5849599479611</v>
+        <v>787.3681265618018</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>764.4906786418346</v>
+        <v>729.2731521683322</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>778.7098881207157</v>
+        <v>601.0136417138483</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>712.8459816805162</v>
+        <v>574.6358074265174</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>601.1971632447626</v>
+        <v>612.5980791205734</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>581.6989226394185</v>
+        <v>628.0656621172227</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>619.1394239838246</v>
+        <v>628.4972320214877</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>628.5451972385943</v>
+        <v>635.7137939683639</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>633.6031365258918</v>
+        <v>638.657027272501</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>650.6263566519692</v>
+        <v>588.2471550526702</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>642.7439130186769</v>
+        <v>517.5109808411094</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>577.5566308223574</v>
+        <v>506.4788680071501</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>512.7035202652905</v>
+        <v>526.942190391253</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>508.0331735393315</v>
+        <v>551.2684362666675</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>525.9361842344674</v>
+        <v>594.294219904782</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>552.6353573004599</v>
+        <v>633.907348304632</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>585.1563267761151</v>
+        <v>620.4080118203592</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>602.8869140633617</v>
+        <v>616.1724441115553</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>588.1311016005384</v>
+        <v>627.8133151039071</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>589.5533439785083</v>
+        <v>608.1386143164025</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>609.6094918803203</v>
+        <v>538.2727689139699</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>599.9858594071839</v>
+        <v>505.9122361980997</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>536.3147831725144</v>
+        <v>528.6802905323214</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>504.3351776782004</v>
+        <v>582.4011266219316</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>525.7611742678989</v>
+        <v>624.0466746556308</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>575.7622970895113</v>
+        <v>625.3951604533654</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>620.3436104414379</v>
+        <v>628.8442364062803</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>622.1416842383292</v>
+        <v>693.1968018072894</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>618.1833492027238</v>
+        <v>726.5643263974653</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>681.8337926655147</v>
+        <v>742.634858834549</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>720.7650095070051</v>
+        <v>724.6854374812131</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>740.3339038017691</v>
+        <v>710.9946883248028</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>724.5888185906892</v>
+        <v>679.3065867299788</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>711.6920182603508</v>
+        <v>633.3040134637429</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>677.3965012623648</v>
+        <v>612.4750860311678</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>629.6730642624198</v>
+        <v>630.4107407806328</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>606.4426304239419</v>
+        <v>671.5204312651792</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>625.6458803272835</v>
+        <v>755.9567528235505</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>663.1930971258839</v>
+        <v>768.565913283652</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>745.3341885995144</v>
+        <v>682.1077193000065</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>771.9696420753621</v>
+        <v>665.9931691220891</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>686.9136084740433</v>
+        <v>713.370938535661</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>664.642486585393</v>
+        <v>732.9872127042165</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>704.5438726163127</v>
+        <v>702.7849130556092</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>735.5504301225437</v>
+        <v>679.5911732821764</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>707.1089782522222</v>
+        <v>651.8260048282229</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>683.3207803467758</v>
+        <v>616.6091899504806</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>652.9571919102466</v>
+        <v>614.7282129128087</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>619.9647008541262</v>
+        <v>617.5581299878843</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>610.3863026897329</v>
+        <v>601.2271277598131</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>620.9121248019756</v>
+        <v>633.0234700869823</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>601.2793005294554</v>
+        <v>665.2176706597288</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>628.1611786841097</v>
+        <v>696.8208902096933</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>659.4523418206393</v>
+        <v>720.1060316999701</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>693.9664579753639</v>
+        <v>700.0520228378377</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>716.0593666951627</v>
+        <v>595.4572535531781</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>704.8647625844637</v>
+        <v>542.6873763995843</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>606.8047980562028</v>
+        <v>517.7471570926571</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>547.3961518983117</v>
+        <v>515.2138031909885</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>523.7399043073481</v>
+        <v>579.8918328804916</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>509.8080836608005</v>
+        <v>652.0935869017421</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>564.8472156657647</v>
+        <v>725.1087462655335</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>642.1954868413025</v>
+        <v>751.688273473917</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>716.3847997436505</v>
+        <v>752.381628582043</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>749.1561494841505</v>
+        <v>758.1868997237393</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>758.2748511946704</v>
+        <v>764.3675273268116</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>757.5313434774102</v>
+        <v>676.5753412808806</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>768.1968725423189</v>
+        <v>584.3782982511243</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>690.9627956293889</v>
+        <v>554.8134177330155</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>596.2624959175287</v>
+        <v>566.4214786474417</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>554.1347239694119</v>
+        <v>593.6195596248126</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>562.2109235366963</v>
+        <v>600.6541907060239</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>587.8425022531815</v>
+        <v>602.9046380578222</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>596.1981650498842</v>
+        <v>636.8085179478271</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>601.3806979503045</v>
+        <v>694.3493011809494</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>627.5574170316531</v>
+        <v>764.6481165758416</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>682.9980595475433</v>
+        <v>795.4192157197326</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="n">
-        <v>753.0297209074206</v>
+        <v>679.7563039448846</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>799.4165607296111</v>
+        <v>570.8048302311397</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>707.2923555424495</v>
+        <v>563.1137909957147</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>576.8449810787502</v>
+        <v>590.0822453146191</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>559.4940244431541</v>
+        <v>567.5942731502346</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>586.1328732247557</v>
+        <v>562.9461235818383</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>573.3555300975297</v>
+        <v>603.9244377829505</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>561.9449844020892</v>
+        <v>654.0513872886322</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>601.6526622267975</v>
+        <v>674.7134228824905</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>648.6828346746165</v>
+        <v>717.2940464264457</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>676.425774003576</v>
+        <v>720.458128448513</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>706.5222479852764</v>
+        <v>706.1284901284068</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>714.7714240912535</v>
+        <v>655.6020551398944</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>707.7376010772696</v>
+        <v>618.5119428162409</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>656.3831656194736</v>
+        <v>606.9915141078468</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>611.5528404576196</v>
+        <v>620.298847495377</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
-        <v>606.8213313749879</v>
+        <v>604.2354627658142</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
-        <v>616.5719122953988</v>
+        <v>630.4516005558867</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
-        <v>602.9741322323332</v>
+        <v>584.4235152807471</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
-        <v>635.4983432970585</v>
+        <v>579.1706227453801</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>606.0950895202097</v>
+        <v>632.1660632529529</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>575.629391430283</v>
+        <v>681.5144743264909</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
-        <v>629.6774859469849</v>
+        <v>699.3721653579712</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
-        <v>682.124256817275</v>
+        <v>679.0449815367481</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="n">
-        <v>711.1286170951132</v>
+        <v>652.0221311149896</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
-        <v>698.4062489063092</v>
+        <v>618.041740042429</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
-        <v>668.0722291808934</v>
+        <v>581.4537717168662</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
-        <v>614.7586523838413</v>
+        <v>572.3464331801154</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="n">
-        <v>568.7174044480514</v>
+        <v>589.750715042868</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="n">
-        <v>549.8918439779743</v>
+        <v>601.0321137277685</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="n">
-        <v>564.3475821990194</v>
+        <v>605.8941200604693</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="n">
-        <v>587.3394520300792</v>
+        <v>556.7777430776459</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="n">
-        <v>606.2682023085983</v>
+        <v>517.0294944439036</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="n">
-        <v>581.6894003850166</v>
+        <v>552.1980057721692</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="n">
-        <v>547.1080274495534</v>
+        <v>571.5077390683803</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="n">
-        <v>569.4530253799712</v>
+        <v>594.8532899523684</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="n">
-        <v>588.8500740694269</v>
+        <v>614.7874512658404</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="n">
-        <v>600.1279235399579</v>
+        <v>632.0662408997464</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="n">
-        <v>608.6710890476752</v>
+        <v>665.3097460602453</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="n">
-        <v>611.265311212037</v>
+        <v>642.1421634057083</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="n">
-        <v>632.7483083153425</v>
+        <v>591.014713353502</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="n">
-        <v>608.7774268745534</v>
+        <v>558.593333593933</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="n">
-        <v>558.9915486604013</v>
+        <v>500.9442811650047</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="n">
-        <v>531.2454256290948</v>
+        <v>490.1576429307966</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="n">
-        <v>499.2442972027789</v>
+        <v>546.5296952073118</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="n">
-        <v>466.6154755487923</v>
+        <v>657.9249798434148</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="n">
-        <v>503.0277520811524</v>
+        <v>762.8685269816629</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="n">
-        <v>607.0309733025283</v>
+        <v>842.7182726222213</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="n">
-        <v>703.0245778935864</v>
+        <v>852.1925422007257</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="n">
-        <v>807.2209194488664</v>
+        <v>795.3346346075705</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="n">
-        <v>853.3659195141468</v>
+        <v>760.5528621623989</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="n">
-        <v>822.5330186115229</v>
+        <v>714.0105274513076</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="n">
-        <v>773.1564923302585</v>
+        <v>630.4289361420956</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="n">
-        <v>722.571339179126</v>
+        <v>633.5043077202158</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="n">
-        <v>687.2492850259846</v>
+        <v>652.2562306751638</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="n">
-        <v>632.547263388858</v>
+        <v>668.6182427373524</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="n">
-        <v>644.6136058495995</v>
+        <v>696.3633453202078</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="n">
-        <v>670.6864840573417</v>
+        <v>697.9368915594364</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="n">
-        <v>685.7111248183401</v>
+        <v>663.8497960037739</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="n">
-        <v>696.2862014564735</v>
+        <v>678.0845796280346</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="n">
-        <v>697.9720731216617</v>
+        <v>684.8552426431525</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="n">
-        <v>709.5386689682641</v>
+        <v>732.5655202442931</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="n">
-        <v>714.0308505962025</v>
+        <v>729.919052154969</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="n">
-        <v>711.1236340757614</v>
+        <v>709.2342675235841</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="n">
-        <v>720.5533682710552</v>
+        <v>670.1185265993672</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="n">
-        <v>723.0713862552989</v>
+        <v>695.2543762191681</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="n">
-        <v>694.0566143984483</v>
+        <v>706.125078250011</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="n">
-        <v>705.7225680563306</v>
+        <v>707.9972226430868</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="n">
-        <v>723.3328544157303</v>
+        <v>717.5021602316747</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="n">
-        <v>730.6573564000018</v>
+        <v>723.8343466543711</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="n">
-        <v>725.0701260971368</v>
+        <v>731.739054124148</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="n">
-        <v>728.9616321891117</v>
+        <v>729.1772238592671</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="n">
-        <v>706.3454572751198</v>
+        <v>692.5343774950079</v>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="n">
-        <v>668.0737559745467</v>
+        <v>621.7055374880829</v>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="n">
-        <v>649.4334852766315</v>
+        <v>557.48895910898</v>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="n">
-        <v>623.026446732581</v>
+        <v>558.9012150966823</v>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="n">
-        <v>576.8346715782968</v>
+        <v>565.4143627996291</v>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="n">
-        <v>546.7296745702015</v>
+        <v>626.6152525696498</v>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="n">
-        <v>572.1984598528138</v>
+        <v>622.092335171601</v>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="n">
-        <v>610.8547100653254</v>
+        <v>647.2727438783181</v>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="n">
-        <v>645.0380362027204</v>
+        <v>656.2218192068485</v>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="n">
-        <v>658.9967783366433</v>
+        <v>688.0932189275768</v>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="n">
-        <v>667.8042314902086</v>
+        <v>710.87716008077</v>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="n">
-        <v>683.6787156008768</v>
+        <v>677.5244586377198</v>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="n">
-        <v>682.9467384638406</v>
+        <v>611.0318589211374</v>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="n">
-        <v>659.6920941812527</v>
+        <v>541.4405045640365</v>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="n">
-        <v>616.1209225165294</v>
+        <v>551.7945286960071</v>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="n">
-        <v>573.4968090191614</v>
+        <v>560.792569395403</v>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="n">
-        <v>554.317176098948</v>
+        <v>527.0959562942039</v>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="n">
-        <v>560.0598117241589</v>
+        <v>540.4179366223616</v>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="n">
-        <v>541.5173197275749</v>
+        <v>593.6662885362693</v>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="n">
-        <v>519.0124175725828</v>
+        <v>640.3448026879346</v>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="n">
-        <v>570.2125570185785</v>
+        <v>742.0810898631203</v>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="n">
-        <v>623.4348031750301</v>
+        <v>749.3731257453646</v>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="n">
-        <v>706.1225234510289</v>
+        <v>682.8187660626099</v>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="n">
-        <v>771.8826700745467</v>
+        <v>672.9484015000935</v>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="n">
-        <v>758.8522749811091</v>
+        <v>635.7225905189807</v>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="n">
-        <v>723.3828174971109</v>
+        <v>650.9249829350665</v>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="n">
-        <v>670.615485965584</v>
+        <v>606.8780460082053</v>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="n">
-        <v>656.8299296895361</v>
+        <v>480.2869772620966</v>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="n">
-        <v>622.4488945228472</v>
+        <v>463.5715562990299</v>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="n">
-        <v>532.1817448278807</v>
+        <v>486.8008695590902</v>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="n">
-        <v>485.5111653067183</v>
+        <v>521.4860833190187</v>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="n">
-        <v>477.1988278611161</v>
+        <v>531.8413201670751</v>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="n">
-        <v>492.9924290915437</v>
+        <v>612.1314568007392</v>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="n">
-        <v>536.7919504469683</v>
+        <v>661.3049320718005</v>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="n">
-        <v>627.3856249545133</v>
+        <v>672.7485382720033</v>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="n">
-        <v>686.5514202920622</v>
+        <v>702.5588352106524</v>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="n">
-        <v>715.3026061581613</v>
+        <v>723.0255648814818</v>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="n">
-        <v>737.9029306189864</v>
+        <v>673.1114282449084</v>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="n">
-        <v>719.0191078325938</v>
+        <v>627.1658480454789</v>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="n">
-        <v>662.8142728746411</v>
+        <v>660.7826460604542</v>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="n">
-        <v>650.492451137211</v>
+        <v>635.8452915511066</v>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="n">
-        <v>686.4012197822831</v>
+        <v>586.5916703740481</v>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="n">
-        <v>630.2223434727239</v>
+        <v>525.709339453897</v>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="n">
-        <v>536.6723543212402</v>
+        <v>553.6914071061005</v>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="n">
-        <v>490.6485265294691</v>
+        <v>600.0465702163069</v>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="n">
-        <v>536.359085655306</v>
+        <v>642.515874555329</v>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="n">
-        <v>615.1697984068392</v>
+        <v>680.4266392568366</v>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="n">
-        <v>688.9726903359588</v>
+        <v>770.7670795414856</v>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="n">
-        <v>739.8293098794397</v>
+        <v>787.7415683979621</v>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="n">
-        <v>794.9472629570664</v>
+        <v>807.4740033536614</v>
       </c>
     </row>
     <row r="501">
       <c r="A501" t="n">
-        <v>766.6666268168569</v>
+        <v>872.529642557879</v>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="n">
-        <v>716.0888742774887</v>
+        <v>758.4621878648363</v>
       </c>
     </row>
     <row r="503">
       <c r="A503" t="n">
-        <v>697.0518600376181</v>
+        <v>746.4874089139926</v>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="n">
-        <v>602.7934895507769</v>
+        <v>798.5453020767181</v>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="n">
-        <v>620.1975466418048</v>
+        <v>773.4108898882823</v>
       </c>
     </row>
     <row r="506">
       <c r="A506" t="n">
-        <v>762.1425150909431</v>
+        <v>777.4825226784401</v>
       </c>
     </row>
     <row r="507">
       <c r="A507" t="n">
-        <v>770.144028165646</v>
+        <v>685.6219396384517</v>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="n">
-        <v>816.9035222011303</v>
+        <v>622.3818588456993</v>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="n">
-        <v>772.2695517115881</v>
+        <v>634.5703691777089</v>
       </c>
     </row>
     <row r="510">
       <c r="A510" t="n">
-        <v>707.0223738262484</v>
+        <v>667.9576783539005</v>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="n">
-        <v>715.8648083971002</v>
+        <v>625.6091921719644</v>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="n">
-        <v>741.7470431163338</v>
+        <v>620.6424482036823</v>
       </c>
     </row>
     <row r="513">
       <c r="A513" t="n">
-        <v>674.7673207354978</v>
+        <v>701.4068263241597</v>
       </c>
     </row>
     <row r="514">
       <c r="A514" t="n">
-        <v>666.4140652274</v>
+        <v>671.6883949212047</v>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="n">
-        <v>729.8597313500181</v>
+        <v>731.1681074781404</v>
       </c>
     </row>
     <row r="516">
       <c r="A516" t="n">
-        <v>750.9773986343475</v>
+        <v>744.1877105279104</v>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="n">
-        <v>817.9591572276763</v>
+        <v>687.2146428371479</v>
       </c>
     </row>
     <row r="518">
       <c r="A518" t="n">
-        <v>803.2839647236187</v>
+        <v>703.9423728724046</v>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="n">
-        <v>693.6571778157372</v>
+        <v>763.5303222247671</v>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="n">
-        <v>690.5979129951447</v>
+        <v>794.8409589225776</v>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="n">
-        <v>742.5914548884975</v>
+        <v>729.9891130473952</v>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="n">
-        <v>765.4709351928659</v>
+        <v>740.7368419740123</v>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="n">
-        <v>763.4488947450109</v>
+        <v>800.0636893609681</v>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="n">
-        <v>811.5734911039567</v>
+        <v>717.5228806873406</v>
       </c>
     </row>
     <row r="525">
       <c r="A525" t="n">
-        <v>786.5566316014565</v>
+        <v>668.019614277739</v>
       </c>
     </row>
     <row r="526">
       <c r="A526" t="n">
-        <v>662.8957271786362</v>
+        <v>667.711313883558</v>
       </c>
     </row>
     <row r="527">
       <c r="A527" t="n">
-        <v>646.9985976655153</v>
+        <v>690.503196153827</v>
       </c>
     </row>
     <row r="528">
       <c r="A528" t="n">
-        <v>693.7431389745825</v>
+        <v>702.9904217999956</v>
       </c>
     </row>
     <row r="529">
       <c r="A529" t="n">
-        <v>771.5889374659923</v>
+        <v>719.2065006296389</v>
       </c>
     </row>
     <row r="530">
       <c r="A530" t="n">
-        <v>773.8228651530221</v>
+        <v>713.7301853902045</v>
       </c>
     </row>
     <row r="531">
       <c r="A531" t="n">
-        <v>746.0435411737194</v>
+        <v>743.2206763797922</v>
       </c>
     </row>
     <row r="532">
       <c r="A532" t="n">
-        <v>748.3113477142638</v>
+        <v>753.4722261813158</v>
       </c>
     </row>
     <row r="533">
       <c r="A533" t="n">
-        <v>769.8094449687574</v>
+        <v>696.3604714471785</v>
       </c>
     </row>
     <row r="534">
       <c r="A534" t="n">
-        <v>757.3764702273706</v>
+        <v>606.7142935547736</v>
       </c>
     </row>
     <row r="535">
       <c r="A535" t="n">
-        <v>634.5329447360086</v>
+        <v>590.213394871796</v>
       </c>
     </row>
     <row r="536">
       <c r="A536" t="n">
-        <v>622.5850778783979</v>
+        <v>602.5503747306402</v>
       </c>
     </row>
     <row r="537">
       <c r="A537" t="n">
-        <v>638.0055354555907</v>
+        <v>617.885847690502</v>
       </c>
     </row>
     <row r="538">
       <c r="A538" t="n">
-        <v>644.7405250531233</v>
+        <v>637.9134679703498</v>
       </c>
     </row>
     <row r="539">
       <c r="A539" t="n">
-        <v>671.4354950219672</v>
+        <v>699.829955994403</v>
       </c>
     </row>
     <row r="540">
       <c r="A540" t="n">
-        <v>647.9926462075127</v>
+        <v>721.2488584816583</v>
       </c>
     </row>
     <row r="541">
       <c r="A541" t="n">
-        <v>626.743889677698</v>
+        <v>694.3337540805032</v>
       </c>
     </row>
     <row r="542">
       <c r="A542" t="n">
-        <v>616.1061903491714</v>
+        <v>766.4790328322511</v>
       </c>
     </row>
     <row r="543">
       <c r="A543" t="n">
-        <v>652.2074752156755</v>
+        <v>740.1278925180463</v>
       </c>
     </row>
     <row r="544">
       <c r="A544" t="n">
-        <v>720.9811650030247</v>
+        <v>699.5701766156799</v>
       </c>
     </row>
     <row r="545">
       <c r="A545" t="n">
-        <v>686.9898038878546</v>
+        <v>713.4260960332881</v>
       </c>
     </row>
     <row r="546">
       <c r="A546" t="n">
-        <v>705.302028887786</v>
+        <v>685.1048870512386</v>
       </c>
     </row>
     <row r="547">
       <c r="A547" t="n">
-        <v>758.0744213900061</v>
+        <v>623.410080269764</v>
       </c>
     </row>
     <row r="548">
       <c r="A548" t="n">
-        <v>748.994589268932</v>
+        <v>579.146299515287</v>
       </c>
     </row>
     <row r="549">
       <c r="A549" t="n">
-        <v>716.0555864329581</v>
+        <v>501.6804215904358</v>
       </c>
     </row>
     <row r="550">
       <c r="A550" t="n">
-        <v>667.9466919956099</v>
+        <v>488.308661250926</v>
       </c>
     </row>
     <row r="551">
       <c r="A551" t="n">
-        <v>615.5564889621132</v>
+        <v>491.5279420083607</v>
       </c>
     </row>
     <row r="552">
       <c r="A552" t="n">
-        <v>573.7436464353323</v>
+        <v>515.5240318744063</v>
       </c>
     </row>
     <row r="553">
       <c r="A553" t="n">
-        <v>567.9805721314324</v>
+        <v>618.0627501530012</v>
       </c>
     </row>
     <row r="554">
       <c r="A554" t="n">
-        <v>575.9558913589444</v>
+        <v>667.0002223991105</v>
       </c>
     </row>
     <row r="555">
       <c r="A555" t="n">
-        <v>577.8457273484037</v>
+        <v>686.7570394903169</v>
       </c>
     </row>
     <row r="556">
       <c r="A556" t="n">
-        <v>600.9217568876579</v>
+        <v>736.9025150070456</v>
       </c>
     </row>
     <row r="557">
       <c r="A557" t="n">
-        <v>664.9658110133032</v>
+        <v>722.4999512910699</v>
       </c>
     </row>
     <row r="558">
       <c r="A558" t="n">
-        <v>737.1200967489813</v>
+        <v>708.3609326359692</v>
       </c>
     </row>
     <row r="559">
       <c r="A559" t="n">
-        <v>690.6886545136217</v>
+        <v>629.4339635537085</v>
       </c>
     </row>
     <row r="560">
       <c r="A560" t="n">
-        <v>604.2474198737295</v>
+        <v>623.6318131474832</v>
       </c>
     </row>
     <row r="561">
       <c r="A561" t="n">
-        <v>633.9068271684027</v>
+        <v>583.857050798656</v>
       </c>
     </row>
     <row r="562">
       <c r="A562" t="n">
-        <v>697.72465244057</v>
+        <v>586.4901438920356</v>
       </c>
     </row>
     <row r="563">
       <c r="A563" t="n">
-        <v>728.4470926917948</v>
+        <v>614.4814608913407</v>
       </c>
     </row>
     <row r="564">
       <c r="A564" t="n">
-        <v>699.5912908603259</v>
+        <v>638.8017051027077</v>
       </c>
     </row>
     <row r="565">
       <c r="A565" t="n">
-        <v>685.2410259004387</v>
+        <v>652.6160187438563</v>
       </c>
     </row>
     <row r="566">
       <c r="A566" t="n">
-        <v>714.3566890288184</v>
+        <v>685.7677540715486</v>
       </c>
     </row>
     <row r="567">
       <c r="A567" t="n">
-        <v>681.1301847204163</v>
+        <v>639.7665979658882</v>
       </c>
     </row>
     <row r="568">
       <c r="A568" t="n">
-        <v>603.10166251071</v>
+        <v>580.3359002204616</v>
       </c>
     </row>
     <row r="569">
       <c r="A569" t="n">
-        <v>578.5924620656147</v>
+        <v>575.4974215133757</v>
       </c>
     </row>
     <row r="570">
       <c r="A570" t="n">
-        <v>613.274219288769</v>
+        <v>589.5281667569066</v>
       </c>
     </row>
     <row r="571">
       <c r="A571" t="n">
-        <v>625.206915559545</v>
+        <v>558.383936028747</v>
       </c>
     </row>
     <row r="572">
       <c r="A572" t="n">
-        <v>635.4373001213389</v>
+        <v>568.026138657217</v>
       </c>
     </row>
     <row r="573">
       <c r="A573" t="n">
-        <v>670.5605484589796</v>
+        <v>605.9902635626599</v>
       </c>
     </row>
     <row r="574">
       <c r="A574" t="n">
-        <v>654.511988658669</v>
+        <v>613.1787850997625</v>
       </c>
     </row>
     <row r="575">
       <c r="A575" t="n">
-        <v>634.6512386555787</v>
+        <v>644.971452264997</v>
       </c>
     </row>
     <row r="576">
       <c r="A576" t="n">
-        <v>648.7486382387146</v>
+        <v>703.9389354231957</v>
       </c>
     </row>
     <row r="577">
       <c r="A577" t="n">
-        <v>645.563540099829</v>
+        <v>672.7943914377761</v>
       </c>
     </row>
     <row r="578">
       <c r="A578" t="n">
-        <v>655.3759678445203</v>
+        <v>672.9428472618793</v>
       </c>
     </row>
     <row r="579">
       <c r="A579" t="n">
-        <v>639.9609188403019</v>
+        <v>617.110612813633</v>
       </c>
     </row>
     <row r="580">
       <c r="A580" t="n">
-        <v>641.6114074508528</v>
+        <v>631.742265406217</v>
       </c>
     </row>
     <row r="581">
       <c r="A581" t="n">
-        <v>626.9253782293163</v>
+        <v>687.3022037050873</v>
       </c>
     </row>
     <row r="582">
       <c r="A582" t="n">
-        <v>635.3951702192262</v>
+        <v>696.5161470037629</v>
       </c>
     </row>
     <row r="583">
       <c r="A583" t="n">
-        <v>671.6680274674331</v>
+        <v>681.8783226435698</v>
       </c>
     </row>
     <row r="584">
       <c r="A584" t="n">
-        <v>753.5335491528485</v>
+        <v>721.127285801515</v>
       </c>
     </row>
     <row r="585">
       <c r="A585" t="n">
-        <v>783.2681285908052</v>
+        <v>681.3206260965217</v>
       </c>
     </row>
     <row r="586">
       <c r="A586" t="n">
-        <v>758.854792130478</v>
+        <v>659.0763645255606</v>
       </c>
     </row>
     <row r="587">
       <c r="A587" t="n">
-        <v>723.5773616472443</v>
+        <v>650.9874514126182</v>
       </c>
     </row>
     <row r="588">
       <c r="A588" t="n">
-        <v>703.5230994986819</v>
+        <v>708.2754083796203</v>
       </c>
     </row>
     <row r="589">
       <c r="A589" t="n">
-        <v>658.3379054584384</v>
+        <v>710.0649441433688</v>
       </c>
     </row>
     <row r="590">
       <c r="A590" t="n">
-        <v>581.0928917123306</v>
+        <v>665.1721356685698</v>
       </c>
     </row>
     <row r="591">
       <c r="A591" t="n">
-        <v>565.9107042809524</v>
+        <v>646.3219422963107</v>
       </c>
     </row>
     <row r="592">
       <c r="A592" t="n">
-        <v>590.9739967918313</v>
+        <v>655.1859191261542</v>
       </c>
     </row>
     <row r="593">
       <c r="A593" t="n">
-        <v>625.8954114583162</v>
+        <v>628.2980647300178</v>
       </c>
     </row>
     <row r="594">
       <c r="A594" t="n">
-        <v>680.1662202158241</v>
+        <v>635.566006053125</v>
       </c>
     </row>
     <row r="595">
       <c r="A595" t="n">
-        <v>659.9570155127594</v>
+        <v>602.6900846918011</v>
       </c>
     </row>
     <row r="596">
       <c r="A596" t="n">
-        <v>705.026609429126</v>
+        <v>625.3031123959545</v>
       </c>
     </row>
     <row r="597">
       <c r="A597" t="n">
-        <v>707.491189427401</v>
+        <v>610.6704805133063</v>
       </c>
     </row>
     <row r="598">
       <c r="A598" t="n">
-        <v>694.2715553390713</v>
+        <v>608.5837769792874</v>
       </c>
     </row>
     <row r="599">
       <c r="A599" t="n">
-        <v>734.7504200841968</v>
+        <v>664.9662099392799</v>
       </c>
     </row>
     <row r="600">
       <c r="A600" t="n">
-        <v>772.5194086303304</v>
+        <v>755.5223442844294</v>
       </c>
     </row>
     <row r="601">
       <c r="A601" t="n">
-        <v>767.8600815416985</v>
+        <v>706.5202550796812</v>
       </c>
     </row>
     <row r="602">
       <c r="A602" t="n">
-        <v>740.4567996763944</v>
+        <v>631.3441319544495</v>
       </c>
     </row>
     <row r="603">
       <c r="A603" t="n">
-        <v>718.4370333789616</v>
+        <v>606.4871875595372</v>
       </c>
     </row>
     <row r="604">
       <c r="A604" t="n">
-        <v>650.174751118243</v>
+        <v>588.9008571350587</v>
       </c>
     </row>
     <row r="605">
       <c r="A605" t="n">
-        <v>551.0190987071724</v>
+        <v>540.7496193700467</v>
       </c>
     </row>
     <row r="606">
       <c r="A606" t="n">
-        <v>531.1700193003048</v>
+        <v>475.9512492797739</v>
       </c>
     </row>
     <row r="607">
       <c r="A607" t="n">
-        <v>560.6949011620372</v>
+        <v>472.1057472121402</v>
       </c>
     </row>
     <row r="608">
       <c r="A608" t="n">
-        <v>600.8853895788775</v>
+        <v>492.6700671501862</v>
       </c>
     </row>
     <row r="609">
       <c r="A609" t="n">
-        <v>683.1204089656353</v>
+        <v>563.4223058551129</v>
       </c>
     </row>
     <row r="610">
       <c r="A610" t="n">
-        <v>749.5483657917248</v>
+        <v>640.4743025109383</v>
       </c>
     </row>
     <row r="611">
       <c r="A611" t="n">
-        <v>758.3478294671977</v>
+        <v>704.3995954166462</v>
       </c>
     </row>
     <row r="612">
       <c r="A612" t="n">
-        <v>725.1488857287995</v>
+        <v>722.964012613545</v>
       </c>
     </row>
     <row r="613">
       <c r="A613" t="n">
-        <v>666.0400210766966</v>
+        <v>690.3419787548728</v>
       </c>
     </row>
     <row r="614">
       <c r="A614" t="n">
-        <v>587.1057209316746</v>
+        <v>604.9584122739589</v>
       </c>
     </row>
     <row r="615">
       <c r="A615" t="n">
-        <v>507.241768939366</v>
+        <v>525.2645033239673</v>
       </c>
     </row>
     <row r="616">
       <c r="A616" t="n">
-        <v>488.5585690091716</v>
+        <v>463.7613226383337</v>
       </c>
     </row>
     <row r="617">
       <c r="A617" t="n">
-        <v>492.0201694810658</v>
+        <v>420.3842657084351</v>
       </c>
     </row>
     <row r="618">
       <c r="A618" t="n">
-        <v>535.53660262628</v>
+        <v>426.299649317059</v>
       </c>
     </row>
     <row r="619">
       <c r="A619" t="n">
-        <v>600.5248316888583</v>
+        <v>468.3357334560014</v>
       </c>
     </row>
     <row r="620">
       <c r="A620" t="n">
-        <v>665.2862097283219</v>
+        <v>505.8473698630905</v>
       </c>
     </row>
     <row r="621">
       <c r="A621" t="n">
-        <v>708.2998785435848</v>
+        <v>556.8994857253529</v>
       </c>
     </row>
     <row r="622">
       <c r="A622" t="n">
-        <v>700.0888394919684</v>
+        <v>549.4628006293851</v>
       </c>
     </row>
     <row r="623">
       <c r="A623" t="n">
-        <v>658.6557443927177</v>
+        <v>540.2691368377077</v>
       </c>
     </row>
     <row r="624">
       <c r="A624" t="n">
-        <v>627.7877335115249</v>
+        <v>554.8283284775266</v>
       </c>
     </row>
     <row r="625">
       <c r="A625" t="n">
-        <v>588.3296280784975</v>
+        <v>572.2719436008674</v>
       </c>
     </row>
     <row r="626">
       <c r="A626" t="n">
-        <v>542.8779779514912</v>
+        <v>518.645876344749</v>
       </c>
     </row>
     <row r="627">
       <c r="A627" t="n">
-        <v>495.5216627413392</v>
+        <v>515.1505159134899</v>
       </c>
     </row>
     <row r="628">
       <c r="A628" t="n">
-        <v>494.472399842607</v>
+        <v>494.5272661591389</v>
       </c>
     </row>
     <row r="629">
       <c r="A629" t="n">
-        <v>504.3349858992201</v>
+        <v>528.4943418211583</v>
       </c>
     </row>
     <row r="630">
       <c r="A630" t="n">
-        <v>562.1204931304078</v>
+        <v>547.6246852713871</v>
       </c>
     </row>
     <row r="631">
       <c r="A631" t="n">
-        <v>651.861909841557</v>
+        <v>519.5819508917907</v>
       </c>
     </row>
     <row r="632">
       <c r="A632" t="n">
-        <v>659.8902344827025</v>
+        <v>523.5954307398742</v>
       </c>
     </row>
     <row r="633">
       <c r="A633" t="n">
-        <v>632.1899794205592</v>
+        <v>506.8503729148688</v>
       </c>
     </row>
     <row r="634">
       <c r="A634" t="n">
-        <v>681.1625365860436</v>
+        <v>516.9439658439501</v>
       </c>
     </row>
     <row r="635">
       <c r="A635" t="n">
-        <v>639.2536221846967</v>
+        <v>584.0640449320063</v>
       </c>
     </row>
     <row r="636">
       <c r="A636" t="n">
-        <v>603.5940078169801</v>
+        <v>647.6682223722605</v>
       </c>
     </row>
     <row r="637">
       <c r="A637" t="n">
-        <v>660.3536763393549</v>
+        <v>642.1641211678661</v>
       </c>
     </row>
     <row r="638">
       <c r="A638" t="n">
-        <v>767.2825442124349</v>
+        <v>657.5419874802151</v>
       </c>
     </row>
     <row r="639">
       <c r="A639" t="n">
-        <v>688.3203538695852</v>
+        <v>679.9540950543133</v>
       </c>
     </row>
     <row r="640">
       <c r="A640" t="n">
-        <v>595.5583287407649</v>
+        <v>653.8814112365685</v>
       </c>
     </row>
     <row r="641">
       <c r="A641" t="n">
-        <v>563.3352271184435</v>
+        <v>632.6745774040887</v>
       </c>
     </row>
     <row r="642">
       <c r="A642" t="n">
-        <v>544.1038106036444</v>
+        <v>600.0934592757972</v>
       </c>
     </row>
     <row r="643">
       <c r="A643" t="n">
-        <v>530.08407310449</v>
+        <v>544.9073174797832</v>
       </c>
     </row>
     <row r="644">
       <c r="A644" t="n">
-        <v>591.6900729257009</v>
+        <v>495.54059424662</v>
       </c>
     </row>
     <row r="645">
       <c r="A645" t="n">
-        <v>679.5315489533209</v>
+        <v>478.8973134980665</v>
       </c>
     </row>
     <row r="646">
       <c r="A646" t="n">
-        <v>746.8131849978477</v>
+        <v>490.9551235036815</v>
       </c>
     </row>
     <row r="647">
       <c r="A647" t="n">
-        <v>742.4772721769273</v>
+        <v>483.2558100812889</v>
       </c>
     </row>
     <row r="648">
       <c r="A648" t="n">
-        <v>689.6528266213977</v>
+        <v>446.5729320130549</v>
       </c>
     </row>
     <row r="649">
       <c r="A649" t="n">
-        <v>644.8486235351538</v>
+        <v>499.4381092226376</v>
       </c>
     </row>
     <row r="650">
       <c r="A650" t="n">
-        <v>617.9216795105731</v>
+        <v>623.0376561385924</v>
       </c>
     </row>
     <row r="651">
       <c r="A651" t="n">
-        <v>583.8843500892494</v>
+        <v>667.3164082418452</v>
       </c>
     </row>
     <row r="652">
       <c r="A652" t="n">
-        <v>529.7355008344198</v>
+        <v>705.08146534155</v>
       </c>
     </row>
     <row r="653">
       <c r="A653" t="n">
-        <v>513.2370519132223</v>
+        <v>677.9686403348251</v>
       </c>
     </row>
     <row r="654">
       <c r="A654" t="n">
-        <v>547.9772181082012</v>
+        <v>605.7137329800071</v>
       </c>
     </row>
     <row r="655">
       <c r="A655" t="n">
-        <v>656.8090171732024</v>
+        <v>571.7759391835102</v>
       </c>
     </row>
     <row r="656">
       <c r="A656" t="n">
-        <v>764.3346253324239</v>
+        <v>556.8859347135913</v>
       </c>
     </row>
     <row r="657">
       <c r="A657" t="n">
-        <v>762.4566304879181</v>
+        <v>552.1671430444712</v>
       </c>
     </row>
     <row r="658">
       <c r="A658" t="n">
-        <v>747.6977385817349</v>
+        <v>521.2289382936319</v>
       </c>
     </row>
     <row r="659">
       <c r="A659" t="n">
-        <v>686.9397762937979</v>
+        <v>518.1358133016829</v>
       </c>
     </row>
     <row r="660">
       <c r="A660" t="n">
-        <v>628.7721962979163</v>
+        <v>551.0293967940356</v>
       </c>
     </row>
     <row r="661">
       <c r="A661" t="n">
-        <v>607.1817026826807</v>
+        <v>605.7437634807457</v>
       </c>
     </row>
     <row r="662">
       <c r="A662" t="n">
-        <v>612.3572348525386</v>
+        <v>672.6303863399608</v>
       </c>
     </row>
     <row r="663">
       <c r="A663" t="n">
-        <v>626.4498518781352</v>
+        <v>659.8936977786138</v>
       </c>
     </row>
     <row r="664">
       <c r="A664" t="n">
-        <v>675.1416722471504</v>
+        <v>579.6233473438974</v>
       </c>
     </row>
     <row r="665">
       <c r="A665" t="n">
-        <v>733.0255303575655</v>
+        <v>517.294982317253</v>
       </c>
     </row>
     <row r="666">
       <c r="A666" t="n">
-        <v>725.4636134586008</v>
+        <v>459.4043857410384</v>
       </c>
     </row>
     <row r="667">
       <c r="A667" t="n">
-        <v>659.2021679321078</v>
+        <v>451.4280621410762</v>
       </c>
     </row>
     <row r="668">
       <c r="A668" t="n">
-        <v>666.1664059997747</v>
+        <v>524.1063512332289</v>
       </c>
     </row>
     <row r="669">
       <c r="A669" t="n">
-        <v>727.879010474453</v>
+        <v>611.0591979584115</v>
       </c>
     </row>
     <row r="670">
       <c r="A670" t="n">
-        <v>786.3580903592151</v>
+        <v>665.1178882458453</v>
       </c>
     </row>
     <row r="671">
       <c r="A671" t="n">
-        <v>781.152257810902</v>
+        <v>704.285096367073</v>
       </c>
     </row>
     <row r="672">
       <c r="A672" t="n">
-        <v>776.9329287114033</v>
+        <v>689.3941454692367</v>
       </c>
     </row>
     <row r="673">
       <c r="A673" t="n">
-        <v>773.1008853193657</v>
+        <v>704.3538652012558</v>
       </c>
     </row>
     <row r="674">
       <c r="A674" t="n">
-        <v>734.3734323416129</v>
+        <v>711.3022218461538</v>
       </c>
     </row>
     <row r="675">
       <c r="A675" t="n">
-        <v>714.6453218658735</v>
+        <v>704.6927521985822</v>
       </c>
     </row>
     <row r="676">
       <c r="A676" t="n">
-        <v>680.6946079190084</v>
+        <v>720.5465567889178</v>
       </c>
     </row>
     <row r="677">
       <c r="A677" t="n">
-        <v>628.7833365898337</v>
+        <v>736.1771755975042</v>
       </c>
     </row>
     <row r="678">
       <c r="A678" t="n">
-        <v>577.8773942207636</v>
+        <v>708.7325406710647</v>
       </c>
     </row>
     <row r="679">
       <c r="A679" t="n">
-        <v>558.6078644799386</v>
+        <v>657.13236563181</v>
       </c>
     </row>
     <row r="680">
       <c r="A680" t="n">
-        <v>609.2410479525938</v>
+        <v>692.9412589985873</v>
       </c>
     </row>
     <row r="681">
       <c r="A681" t="n">
-        <v>647.8538131931373</v>
+        <v>712.4666393712573</v>
       </c>
     </row>
     <row r="682">
       <c r="A682" t="n">
-        <v>594.7669224185006</v>
+        <v>687.7507885190539</v>
       </c>
     </row>
     <row r="683">
       <c r="A683" t="n">
-        <v>532.6374775356726</v>
+        <v>688.8425121069872</v>
       </c>
     </row>
     <row r="684">
       <c r="A684" t="n">
-        <v>522.4180511347072</v>
+        <v>669.0045384970631</v>
       </c>
     </row>
     <row r="685">
       <c r="A685" t="n">
-        <v>547.5409777437221</v>
+        <v>608.5724387813229</v>
       </c>
     </row>
     <row r="686">
       <c r="A686" t="n">
-        <v>578.9155986569767</v>
+        <v>594.5332556597691</v>
       </c>
     </row>
     <row r="687">
       <c r="A687" t="n">
-        <v>617.722195021031</v>
+        <v>567.4719669060551</v>
       </c>
     </row>
     <row r="688">
       <c r="A688" t="n">
-        <v>681.8324072712016</v>
+        <v>563.9752041165025</v>
       </c>
     </row>
     <row r="689">
       <c r="A689" t="n">
-        <v>750.3596525529019</v>
+        <v>577.3459634887672</v>
       </c>
     </row>
     <row r="690">
       <c r="A690" t="n">
-        <v>731.1071528308162</v>
+        <v>596.9838590984295</v>
       </c>
     </row>
     <row r="691">
       <c r="A691" t="n">
-        <v>720.2985391422771</v>
+        <v>623.9004272229067</v>
       </c>
     </row>
     <row r="692">
       <c r="A692" t="n">
-        <v>647.1895652995272</v>
+        <v>634.5252322325337</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="n">
+        <v>649.2710403248338</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="n">
+        <v>688.0087011174965</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="n">
+        <v>716.7100127648496</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="n">
+        <v>734.6750932533155</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="n">
+        <v>719.1029960591209</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="n">
+        <v>671.4567598989447</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="n">
+        <v>649.7613437086329</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="n">
+        <v>606.6792191082868</v>
       </c>
     </row>
   </sheetData>

</xml_diff>